<commit_message>
update code reg ssepration
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="76">
   <si>
     <t>Sr No</t>
   </si>
@@ -27,82 +27,88 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Total_time</t>
+  </si>
+  <si>
+    <t>Test  Sub scenario</t>
+  </si>
+  <si>
+    <t>Open Browser</t>
+  </si>
+  <si>
+    <t>Login_page</t>
+  </si>
+  <si>
+    <t>Application_page</t>
+  </si>
+  <si>
+    <t>Data Discovery</t>
+  </si>
+  <si>
     <t>Account Card</t>
   </si>
   <si>
-    <t>Open Browser</t>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Vizpod</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Data Ingest</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Rule Group</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Data Profile</t>
+  </si>
+  <si>
+    <t>Compare Result</t>
+  </si>
+  <si>
+    <t>Data Quality</t>
+  </si>
+  <si>
+    <t>Data Preparation</t>
+  </si>
+  <si>
+    <t>Datapod</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t>Data Renconciliation</t>
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>Login_page</t>
-  </si>
-  <si>
-    <t>Application_page</t>
-  </si>
-  <si>
-    <t>Data Discovery</t>
-  </si>
-  <si>
-    <t>Data Visualization</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>Vizpod</t>
-  </si>
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>Data Ingest</t>
-  </si>
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>Rule Group</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Data Profile</t>
-  </si>
-  <si>
-    <t>Compare Result</t>
-  </si>
-  <si>
-    <t>Data Quality</t>
-  </si>
-  <si>
-    <t>Data Preparation</t>
-  </si>
-  <si>
-    <t>Datapod</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>Expression</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Map</t>
-  </si>
-  <si>
-    <t>Relation</t>
-  </si>
-  <si>
-    <t>Data Renconciliation</t>
   </si>
   <si>
     <t>Business Rule</t>
@@ -247,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -275,11 +281,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -336,7 +337,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -353,19 +354,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,10 +447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38:AG38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -476,8 +473,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="0" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -486,23 +491,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1078.0</v>
-      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -512,13 +509,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,13 +523,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D4" t="n">
         <v>0.0</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,408 +537,430 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>1064.0</v>
+        <v>1166.0</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1544.0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1161.0</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1090.0</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>1109.0</v>
+        <v>1169.0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>1115.0</v>
+        <v>1086.0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
-        <v>1079.0</v>
+        <v>1066.0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D11" t="n">
-        <v>1326.0</v>
+        <v>1079.0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>1342</v>
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1106.0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>1425</v>
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1269.0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>1080</v>
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1255.0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1252.0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1068.0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>1076</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>1077</v>
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>14</v>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1076.0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>15</v>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1124.0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>1144</v>
+        <v>21</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>1348</v>
+        <v>22</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>1283</v>
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1121.0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>1330</v>
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1358.0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>1281</v>
+        <v>25</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1304.0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>1355</v>
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1359.0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1330.0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1354.0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1370.0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1300.0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1088.0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1071.0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>16</v>
@@ -955,239 +968,311 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1321.0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1104.0</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1280.0</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>1366</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>1309</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>37</v>
       </c>
+      <c r="C51" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>1268</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>1346</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="C53" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>1314</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="C54" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>1352</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="C55" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>1260</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>1079</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
-        <v>56</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>42</v>
+        <v>54</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
-        <v>57</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="C59" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>1303</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>45</v>
+        <v>58</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
-        <v>62</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>44</v>
+        <v>60</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
-        <v>63</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
-        <v>67</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>44</v>
+        <v>65</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>49</v>
@@ -1195,7 +1280,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>50</v>
@@ -1203,7 +1288,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>51</v>
@@ -1211,15 +1296,15 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="B75" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>53</v>
@@ -1227,7 +1312,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>54</v>
@@ -1235,39 +1320,39 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="B78" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="0" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
-        <v>78</v>
-      </c>
-      <c r="B79" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="0" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
-        <v>79</v>
-      </c>
-      <c r="B80" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="B81" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>59</v>
@@ -1275,7 +1360,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>60</v>
@@ -1283,7 +1368,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>61</v>
@@ -1291,7 +1376,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>62</v>
@@ -1299,7 +1384,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>63</v>
@@ -1307,7 +1392,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>64</v>
@@ -1315,21 +1400,37 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="n">
         <v>90</v>
       </c>
     </row>
@@ -1352,7 +1453,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="D38:AG38 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1368,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1"/>
     </row>
@@ -1379,22 +1480,22 @@
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>68</v>
+      <c r="B2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>68</v>
+      <c r="B3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,10 +1503,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,10 +1514,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,7 +1566,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="L13" s="7"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">

</xml_diff>